<commit_message>
OO-2364 update excel question import example, add k-prim section for 2.1 import
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
+++ b/src/main/resources/org/olat/ims/qti21/questionimport/qti-import-metadata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="0" windowWidth="30700" windowHeight="27140" tabRatio="500"/>
+    <workbookView xWindow="8400" yWindow="0" windowWidth="36080" windowHeight="30860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Import" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
   <si>
     <t>Typ</t>
   </si>
@@ -310,6 +310,33 @@
   </si>
   <si>
     <t>Optional</t>
+  </si>
+  <si>
+    <t>KPRIM</t>
+  </si>
+  <si>
+    <t>Fragetpy: K-Prim</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Eine wahre Antwort</t>
+  </si>
+  <si>
+    <t>Fussball: Weltmeister</t>
+  </si>
+  <si>
+    <t>Prüfen Sie die Weltmeiser kennen</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Die folgenden Länder haben die Fussball Weltmeistertitel bereits mehr als einmal gewonnen.</t>
   </si>
 </sst>
 </file>
@@ -436,7 +463,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -454,6 +481,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -516,7 +545,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Ausgabe" xfId="16" builtinId="21"/>
     <cellStyle name="Besuchter Link" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="5" builtinId="9" hidden="1"/>
@@ -536,6 +565,7 @@
     <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Erklärender Text" xfId="1" builtinId="53"/>
     <cellStyle name="Link" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="4" builtinId="8" hidden="1"/>
@@ -555,6 +585,7 @@
     <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -884,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1581,6 +1612,105 @@
         <v>32</v>
       </c>
     </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="30">
+      <c r="A70" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="45">
+      <c r="A71" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" s="7">
+        <v>1</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>